<commit_message>
Experiments with how excel_to_go might work
</commit_message>
<xml_diff>
--- a/spec/test.xlsx
+++ b/spec/test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Documents/github/excel_to_code/spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACCB139-00FF-BD49-A922-7AA6D54ED2D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5440" windowWidth="28040" windowHeight="17440" xr2:uid="{5CFDD89D-F887-804F-8310-58AEC808B261}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -395,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE5C522-2B25-B842-9387-18CCE45A12AB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -419,15 +420,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -435,7 +440,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -443,7 +448,7 @@
         <v>0.999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -451,7 +456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -459,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -468,7 +473,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -477,7 +482,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -486,7 +491,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -495,7 +500,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>

</xml_diff>